<commit_message>
update scripts after detailed screening + add new packages
</commit_message>
<xml_diff>
--- a/dq-checks.xlsx
+++ b/dq-checks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Integrity</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Disagreement with gold standard</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -515,368 +518,473 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B4">
+        <v>1001</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B5">
+        <v>1002</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B6">
+        <v>1003</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B8">
+        <v>1004</v>
+      </c>
+      <c r="E8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
+      <c r="B9">
+        <v>1005</v>
+      </c>
+      <c r="E9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B11">
+        <v>1006</v>
+      </c>
+      <c r="E11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B12">
+        <v>1007</v>
+      </c>
+      <c r="E12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B13">
+        <v>1008</v>
+      </c>
+      <c r="E13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
-      <c r="D17" t="s">
+      <c r="B17">
+        <v>2001</v>
+      </c>
+      <c r="E17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
-      <c r="D19" t="s">
+      <c r="B19">
+        <v>2002</v>
+      </c>
+      <c r="E19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="B20">
+        <v>2003</v>
+      </c>
+      <c r="E20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
-      <c r="D21" t="s">
+      <c r="B21">
+        <v>2004</v>
+      </c>
+      <c r="E21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
-      <c r="D22" t="s">
+      <c r="B22">
+        <v>2005</v>
+      </c>
+      <c r="E22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>14</v>
       </c>
-      <c r="D26" t="s">
+      <c r="B26">
+        <v>3001</v>
+      </c>
+      <c r="E26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15</v>
       </c>
-      <c r="D27" t="s">
+      <c r="B27">
+        <v>3002</v>
+      </c>
+      <c r="E27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>16</v>
       </c>
-      <c r="D28" t="s">
+      <c r="B28">
+        <v>3003</v>
+      </c>
+      <c r="E28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>17</v>
       </c>
-      <c r="D29" t="s">
+      <c r="B29">
+        <v>3004</v>
+      </c>
+      <c r="E29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>18</v>
       </c>
-      <c r="D30" t="s">
+      <c r="B30">
+        <v>3005</v>
+      </c>
+      <c r="E30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>19</v>
       </c>
-      <c r="D31" t="s">
+      <c r="B31">
+        <v>3006</v>
+      </c>
+      <c r="E31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>20</v>
       </c>
-      <c r="D32" t="s">
+      <c r="B32">
+        <v>3007</v>
+      </c>
+      <c r="E32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>21</v>
       </c>
-      <c r="D34" t="s">
+      <c r="B34">
+        <v>3008</v>
+      </c>
+      <c r="E34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>22</v>
       </c>
-      <c r="D35" t="s">
+      <c r="B35">
+        <v>3009</v>
+      </c>
+      <c r="E35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>23</v>
       </c>
-      <c r="D39" t="s">
+      <c r="B39">
+        <v>4001</v>
+      </c>
+      <c r="E39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>24</v>
       </c>
-      <c r="D40" t="s">
+      <c r="B40">
+        <v>4002</v>
+      </c>
+      <c r="E40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>25</v>
       </c>
-      <c r="D41" t="s">
+      <c r="B41">
+        <v>4003</v>
+      </c>
+      <c r="E41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>26</v>
       </c>
-      <c r="D42" t="s">
+      <c r="B42">
+        <v>4004</v>
+      </c>
+      <c r="E42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>27</v>
       </c>
-      <c r="D43" t="s">
+      <c r="B43">
+        <v>4005</v>
+      </c>
+      <c r="E43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>28</v>
       </c>
-      <c r="D44" t="s">
+      <c r="B44">
+        <v>4006</v>
+      </c>
+      <c r="E44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>29</v>
       </c>
-      <c r="D46" t="s">
+      <c r="B46">
+        <v>4007</v>
+      </c>
+      <c r="E46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>30</v>
       </c>
-      <c r="D47" t="s">
+      <c r="B47">
+        <v>4008</v>
+      </c>
+      <c r="E47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>31</v>
       </c>
-      <c r="D48" t="s">
+      <c r="B48">
+        <v>4009</v>
+      </c>
+      <c r="E48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>32</v>
       </c>
-      <c r="D50" t="s">
+      <c r="B50">
+        <v>4010</v>
+      </c>
+      <c r="E50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>33</v>
       </c>
-      <c r="D51" t="s">
+      <c r="B51">
+        <v>4011</v>
+      </c>
+      <c r="E51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>34</v>
       </c>
-      <c r="D52" t="s">
+      <c r="B52">
+        <v>4012</v>
+      </c>
+      <c r="E52" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>